<commit_message>
Xray Test Execution Entegration Done
</commit_message>
<xml_diff>
--- a/output/xray_import.xlsx
+++ b/output/xray_import.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TC-001 Verify the form page loads successfully</t>
+          <t>TC-001 Verify page loads successfully</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>The form page loads completely without errors, all UI elements including username input, password input, submit button, and links are visible and enabled</t>
+          <t>The form page loads completely without errors, all UI elements including username input, password input, and submit button are visible and enabled</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TC-002 Fill all mandatory input fields on the form page</t>
+          <t>TC-002 Fill all mandatory input fields with valid data</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Both input fields accept the input without errors and display the entered values correctly</t>
+          <t>Both fields accept the input without errors or warnings</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TC-002 Fill all mandatory input fields on the form page</t>
+          <t>TC-002 Fill all mandatory input fields with valid data</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Both input fields accept the input without errors and display the entered values correctly</t>
+          <t>Both fields accept the input without errors or warnings</t>
         </is>
       </c>
     </row>
@@ -599,17 +599,17 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>All mandatory fields are filled with valid data</t>
+          <t>Username and password fields are filled with valid data</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>Click on the submit button</t>
+          <t>Click the submit button</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>The form is submitted successfully without client-side validation errors</t>
+          <t>Form is submitted successfully and a success response or confirmation message is displayed</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Form has been submitted with valid data</t>
+          <t>Form submitted with valid data</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>Observe the response after form submission</t>
+          <t>Observe the response after submission</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>A success message or confirmation page is displayed indicating the form was submitted successfully</t>
+          <t>A success message or redirection to a confirmation page is displayed indicating successful submission</t>
         </is>
       </c>
     </row>
@@ -658,7 +658,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TC-005 Verify that all links on the form page are clickable</t>
+          <t>TC-005 Submit the form with empty username field</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -668,22 +668,2390 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Form page is loaded successfully</t>
+          <t>Password field is filled with valid data, username field is empty</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>Click each link on the form page one by one</t>
+          <t>Leave username field empty</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Each link navigates to the expected destination without errors or broken links</t>
+          <t>Form submission is blocked, an error message indicating "Username is required" is displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TC-005 Submit the form with empty username field</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>Password field is filled with valid data, username field is empty</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid password</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Form submission is blocked, an error message indicating "Username is required" is displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TC-005 Submit the form with empty username field</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Password field is filled with valid data, username field is empty</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>Form submission is blocked, an error message indicating "Username is required" is displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TC-006 Submit the form with empty password field</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>Username field is filled with valid data, password field is empty</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Form submission is blocked, an error message indicating "Password is required" is displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TC-006 Submit the form with empty password field</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>Username field is filled with valid data, password field is empty</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>Leave password field empty</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>Form submission is blocked, an error message indicating "Password is required" is displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TC-006 Submit the form with empty password field</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>Username field is filled with valid data, password field is empty</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>Form submission is blocked, an error message indicating "Password is required" is displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TC-007 Submit the form with both username and password fields empty</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>Both username and password fields are empty</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>Leave username and password fields empty</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Form submission is blocked, error messages indicating both fields are required are displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TC-007 Submit the form with both username and password fields empty</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>Both username and password fields are empty</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>Form submission is blocked, error messages indicating both fields are required are displayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>TC-008 Enter invalid characters in username field</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>Enter invalid characters (e.g., special symbols like @#$%) in username field</t>
+        </is>
+      </c>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating invalid username format is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TC-008 Enter invalid characters in username field</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid password</t>
+        </is>
+      </c>
+      <c r="G16" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating invalid username format is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>TC-008 Enter invalid characters in username field</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G17" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating invalid username format is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TC-009 Enter invalid characters in password field</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username</t>
+        </is>
+      </c>
+      <c r="G18" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating invalid password format or length is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>TC-009 Enter invalid characters in password field</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>Enter invalid characters or too short password (e.g., less than minimum length)</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating invalid password format or length is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>TC-009 Enter invalid characters in password field</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating invalid password format or length is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>TC-010 Submit form with username at minimum length boundary</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, minimum username length is known (e.g., 3 characters)</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>Enter username with minimum allowed length (e.g., 3 characters)</t>
+        </is>
+      </c>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TC-010 Submit form with username at minimum length boundary</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, minimum username length is known (e.g., 3 characters)</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid password</t>
+        </is>
+      </c>
+      <c r="G22" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>TC-010 Submit form with username at minimum length boundary</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, minimum username length is known (e.g., 3 characters)</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>TC-011 Submit form with username below minimum length boundary</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, minimum username length is known</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>Enter username with length less than minimum allowed (e.g., 2 characters)</t>
+        </is>
+      </c>
+      <c r="G24" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating username is too short is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>TC-011 Submit form with username below minimum length boundary</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, minimum username length is known</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid password</t>
+        </is>
+      </c>
+      <c r="G25" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating username is too short is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>TC-011 Submit form with username below minimum length boundary</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, minimum username length is known</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G26" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating username is too short is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>TC-012 Submit form with password at maximum length boundary</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, maximum password length is known (e.g., 20 characters)</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username</t>
+        </is>
+      </c>
+      <c r="G27" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>TC-012 Submit form with password at maximum length boundary</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, maximum password length is known (e.g., 20 characters)</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>Enter password with maximum allowed length (e.g., 20 characters)</t>
+        </is>
+      </c>
+      <c r="G28" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>TC-012 Submit form with password at maximum length boundary</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, maximum password length is known (e.g., 20 characters)</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>TC-013 Submit form with password exceeding maximum length boundary</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, maximum password length is known</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating password is too long is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>TC-013 Submit form with password exceeding maximum length boundary</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, maximum password length is known</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>Enter password exceeding maximum allowed length (e.g., 21 characters)</t>
+        </is>
+      </c>
+      <c r="G31" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating password is too long is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>TC-013 Submit form with password exceeding maximum length boundary</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, maximum password length is known</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>Validation error message indicating password is too long is displayed, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>TC-014 Verify form handles SQL injection attempt in username field</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>Enter SQL injection string (e.g., "' OR '1'='1") in username field</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="inlineStr">
+        <is>
+          <t>Form rejects input, displays validation error or sanitizes input, no backend error or data breach occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>TC-014 Verify form handles SQL injection attempt in username field</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid password</t>
+        </is>
+      </c>
+      <c r="G34" s="2" t="inlineStr">
+        <is>
+          <t>Form rejects input, displays validation error or sanitizes input, no backend error or data breach occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>TC-014 Verify form handles SQL injection attempt in username field</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G35" s="2" t="inlineStr">
+        <is>
+          <t>Form rejects input, displays validation error or sanitizes input, no backend error or data breach occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>TC-015 Verify form handles script injection attempt in password field</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username</t>
+        </is>
+      </c>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>Form rejects input, displays validation error or sanitizes input, no script execution occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>TC-015 Verify form handles script injection attempt in password field</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>Enter script injection string (e.g., "&lt;script&gt;alert('test')&lt;/script&gt;") in password field</t>
+        </is>
+      </c>
+      <c r="G37" s="2" t="inlineStr">
+        <is>
+          <t>Form rejects input, displays validation error or sanitizes input, no script execution occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>TC-015 Verify form handles script injection attempt in password field</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G38" s="2" t="inlineStr">
+        <is>
+          <t>Form rejects input, displays validation error or sanitizes input, no script execution occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>TC-016 Verify navigation links (anchor tags) are clickable and redirect correctly</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>Click each anchor link on the page one by one</t>
+        </is>
+      </c>
+      <c r="G39" s="2" t="inlineStr">
+        <is>
+          <t>Each link navigates to the expected page or section without errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>TC-017 Verify form submission with maximum allowed input length for username and password</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>Maximum input lengths are known</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>Enter username with maximum allowed length</t>
+        </is>
+      </c>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without errors or truncation</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>TC-017 Verify form submission with maximum allowed input length for username and password</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>Maximum input lengths are known</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>Enter password with maximum allowed length</t>
+        </is>
+      </c>
+      <c r="G41" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without errors or truncation</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>TC-017 Verify form submission with maximum allowed input length for username and password</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>Maximum input lengths are known</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G42" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without errors or truncation</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>TC-018 Verify form submission with minimum allowed input length for username and password</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>Minimum input lengths are known</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>Enter username with minimum allowed length</t>
+        </is>
+      </c>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>TC-018 Verify form submission with minimum allowed input length for username and password</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>Minimum input lengths are known</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>Enter password with minimum allowed length</t>
+        </is>
+      </c>
+      <c r="G44" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>TC-018 Verify form submission with minimum allowed input length for username and password</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>Minimum input lengths are known</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G45" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TC-019 Verify form does not accept whitespace-only input in username and password fields</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>Enter spaces or tabs only in username field</t>
+        </is>
+      </c>
+      <c r="G46" s="2" t="inlineStr">
+        <is>
+          <t>Validation error messages indicating fields cannot be whitespace only, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>TC-019 Verify form does not accept whitespace-only input in username and password fields</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>Enter spaces or tabs only in password field</t>
+        </is>
+      </c>
+      <c r="G47" s="2" t="inlineStr">
+        <is>
+          <t>Validation error messages indicating fields cannot be whitespace only, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TC-019 Verify form does not accept whitespace-only input in username and password fields</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>Validation error messages indicating fields cannot be whitespace only, form submission is blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TC-020 Verify error message disappears after correcting invalid input</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, invalid input entered previously</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>Enter invalid username or password to trigger error message</t>
+        </is>
+      </c>
+      <c r="G49" s="2" t="inlineStr">
+        <is>
+          <t>Error message disappears immediately or after form validation, allowing form submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>TC-020 Verify error message disappears after correcting invalid input</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded, invalid input entered previously</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>Correct the input to valid data</t>
+        </is>
+      </c>
+      <c r="G50" s="2" t="inlineStr">
+        <is>
+          <t>Error message disappears immediately or after form validation, allowing form submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>TC-021 Verify form handles server error gracefully on submission</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>Server is configured to simulate an error response on form submission</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username and password</t>
+        </is>
+      </c>
+      <c r="G51" s="2" t="inlineStr">
+        <is>
+          <t>User is shown a friendly error message indicating submission failure, no application crash occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>TC-021 Verify form handles server error gracefully on submission</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>Server is configured to simulate an error response on form submission</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G52" s="2" t="inlineStr">
+        <is>
+          <t>User is shown a friendly error message indicating submission failure, no application crash occurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TC-022 Verify form handles network timeout during submission</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>Network conditions simulate timeout or slow response</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username and password</t>
+        </is>
+      </c>
+      <c r="G53" s="2" t="inlineStr">
+        <is>
+          <t>User is informed of network timeout or retry option, form does not freeze or crash</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>TC-022 Verify form handles network timeout during submission</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>Network conditions simulate timeout or slow response</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G54" s="2" t="inlineStr">
+        <is>
+          <t>User is informed of network timeout or retry option, form does not freeze or crash</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>TC-023 Verify form prevents multiple submissions on double-click of submit button</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>Enter valid username and password</t>
+        </is>
+      </c>
+      <c r="G55" s="2" t="inlineStr">
+        <is>
+          <t>Only one form submission is processed, multiple submissions are prevented</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TC-023 Verify form prevents multiple submissions on double-click of submit button</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>Doubleclick the submit button rapidly</t>
+        </is>
+      </c>
+      <c r="G56" s="2" t="inlineStr">
+        <is>
+          <t>Only one form submission is processed, multiple submissions are prevented</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>TC-024 Verify form resets input fields after successful submission</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>Form submitted successfully</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>Submit form with valid data</t>
+        </is>
+      </c>
+      <c r="G57" s="2" t="inlineStr">
+        <is>
+          <t>Username and password fields are cleared/reset after successful submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>TC-025 Verify tab order and keyboard accessibility of form fields and buttons</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>Use keyboard tab key to navigate through username input, password input, and submit button</t>
+        </is>
+      </c>
+      <c r="G58" s="2" t="inlineStr">
+        <is>
+          <t>Focus moves in logical order, all elements are accessible via keyboard</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>TC-026 Verify password input field masks entered characters</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>Enter password in password input field</t>
+        </is>
+      </c>
+      <c r="G59" s="2" t="inlineStr">
+        <is>
+          <t>Characters are masked (e.g., shown as dots or asterisks) and not visible as plain text</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>TC-027 Verify form submission with special but allowed characters in username and password</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>Enter username and password containing allowed special characters (e.g., underscore, hyphen)</t>
+        </is>
+      </c>
+      <c r="G60" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>TC-027 Verify form submission with special but allowed characters in username and password</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G61" s="2" t="inlineStr">
+        <is>
+          <t>Form submits successfully without validation errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>TC-028 Verify form does not accept input exceeding maximum allowed length in username and password fields</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>Maximum input lengths are known</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>Attempt to enter input longer than maximum allowed length in username and password fields</t>
+        </is>
+      </c>
+      <c r="G62" s="2" t="inlineStr">
+        <is>
+          <t>Input is truncated or prevented from entering beyond max length, no errors occur on typing</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>TC-029 Verify error message is displayed in correct language/localization (if applicable)</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>Application localization is enabled and set to a specific language</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>Trigger validation error by submitting empty username or password</t>
+        </is>
+      </c>
+      <c r="G63" s="2" t="inlineStr">
+        <is>
+          <t>Error message is displayed in the selected language correctly</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>TC-030 Verify form submission with leading and trailing spaces in username and password fields</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>Enter username and password with leading and trailing spaces</t>
+        </is>
+      </c>
+      <c r="G64" s="2" t="inlineStr">
+        <is>
+          <t>Spaces are trimmed automatically or validation error is shown, form submission behaves as expected</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>TC-030 Verify form submission with leading and trailing spaces in username and password fields</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G65" s="2" t="inlineStr">
+        <is>
+          <t>Spaces are trimmed automatically or validation error is shown, form submission behaves as expected</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>TC-031 Verify form handles browser back and forward navigation without data loss</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded and partially filled</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>Enter data in username and password fields</t>
+        </is>
+      </c>
+      <c r="G66" s="2" t="inlineStr">
+        <is>
+          <t>Previously entered data is retained or user is prompted accordingly</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>TC-031 Verify form handles browser back and forward navigation without data loss</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded and partially filled</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>Navigate away using browser back button</t>
+        </is>
+      </c>
+      <c r="G67" s="2" t="inlineStr">
+        <is>
+          <t>Previously entered data is retained or user is prompted accordingly</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>TC-031 Verify form handles browser back and forward navigation without data loss</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded and partially filled</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>Navigate forward to the form page again</t>
+        </is>
+      </c>
+      <c r="G68" s="2" t="inlineStr">
+        <is>
+          <t>Previously entered data is retained or user is prompted accordingly</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>TC-032 Verify form submission with copy-paste input in username and password fields</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>Copy valid username and password from external source</t>
+        </is>
+      </c>
+      <c r="G69" s="2" t="inlineStr">
+        <is>
+          <t>Form accepts pasted input and submits successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>TC-032 Verify form submission with copy-paste input in username and password fields</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>Paste into respective fields</t>
+        </is>
+      </c>
+      <c r="G70" s="2" t="inlineStr">
+        <is>
+          <t>Form accepts pasted input and submits successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>TC-032 Verify form submission with copy-paste input in username and password fields</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>Form page is loaded</t>
+        </is>
+      </c>
+      <c r="F71" s="2" t="inlineStr">
+        <is>
+          <t>Click submit button</t>
+        </is>
+      </c>
+      <c r="G71" s="2" t="inlineStr">
+        <is>
+          <t>Form accepts pasted input and submits successfully</t>
         </is>
       </c>
     </row>

</xml_diff>